<commit_message>
modif dictionnaire de donnees + mcd papyrus
</commit_message>
<xml_diff>
--- a/persistance_des_données/developper_des_composants/papyrus/dictionnaire_de_donnees.xlsx
+++ b/persistance_des_données/developper_des_composants/papyrus/dictionnaire_de_donnees.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="73">
   <si>
     <t>CODE</t>
   </si>
@@ -138,6 +138,12 @@
     <t xml:space="preserve">Identifiant de la commande</t>
   </si>
   <si>
+    <t>numCommande</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Numéro de la commande</t>
+  </si>
+  <si>
     <t>dateCommande</t>
   </si>
   <si>
@@ -157,6 +163,12 @@
   </si>
   <si>
     <t xml:space="preserve">Indentifiant d'une ligne de la commande</t>
+  </si>
+  <si>
+    <t>numLigneCommande</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Numéro de la ligne de la commande</t>
   </si>
   <si>
     <t>qteLigneCommande</t>
@@ -788,7 +800,7 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac">
   <sheetViews>
-    <sheetView topLeftCell="A7" zoomScale="100" workbookViewId="0">
+    <sheetView zoomScale="100" workbookViewId="0">
       <selection activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
@@ -1071,15 +1083,15 @@
         <v>8</v>
       </c>
     </row>
-    <row r="18" ht="28.5">
+    <row r="18" ht="14.25">
       <c r="A18" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="B18" s="5" t="s">
+      <c r="B18" s="3" t="s">
         <v>42</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>43</v>
+        <v>7</v>
       </c>
       <c r="D18" s="3"/>
       <c r="E18" s="4" t="s">
@@ -1088,19 +1100,17 @@
     </row>
     <row r="19" ht="28.5">
       <c r="A19" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="B19" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="B19" s="5" t="s">
+      <c r="C19" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="C19" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="D19" s="3">
-        <v>50</v>
-      </c>
+      <c r="D19" s="3"/>
       <c r="E19" s="4" t="s">
-        <v>38</v>
+        <v>8</v>
       </c>
     </row>
     <row r="20" ht="28.5">
@@ -1111,11 +1121,13 @@
         <v>47</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D20" s="3"/>
+        <v>13</v>
+      </c>
+      <c r="D20" s="3">
+        <v>50</v>
+      </c>
       <c r="E20" s="4" t="s">
-        <v>8</v>
+        <v>38</v>
       </c>
     </row>
     <row r="21" ht="28.5">
@@ -1141,37 +1153,37 @@
         <v>51</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>52</v>
+        <v>7</v>
       </c>
       <c r="D22" s="3"/>
       <c r="E22" s="4" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="23" ht="14.25">
+    <row r="23" ht="28.5">
       <c r="A23" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="B23" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="B23" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="C23" s="4" t="s">
+      <c r="C23" s="3" t="s">
         <v>7</v>
       </c>
       <c r="D23" s="3"/>
       <c r="E23" s="4" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="24" ht="14.25">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="24" ht="28.5">
       <c r="A24" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="B24" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="B24" s="3" t="s">
+      <c r="C24" s="3" t="s">
         <v>56</v>
-      </c>
-      <c r="C24" s="3" t="s">
-        <v>43</v>
       </c>
       <c r="D24" s="3"/>
       <c r="E24" s="4" t="s">
@@ -1185,27 +1197,27 @@
       <c r="B25" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="C25" s="3" t="s">
-        <v>52</v>
+      <c r="C25" s="4" t="s">
+        <v>7</v>
       </c>
       <c r="D25" s="3"/>
-      <c r="E25" s="3" t="s">
-        <v>8</v>
+      <c r="E25" s="4" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="26" ht="14.25">
       <c r="A26" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="B26" s="4" t="s">
+      <c r="B26" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="C26" s="4" t="s">
-        <v>52</v>
+      <c r="C26" s="3" t="s">
+        <v>45</v>
       </c>
       <c r="D26" s="3"/>
-      <c r="E26" s="3" t="s">
-        <v>38</v>
+      <c r="E26" s="4" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="27" ht="14.25">
@@ -1215,12 +1227,12 @@
       <c r="B27" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="C27" s="4" t="s">
-        <v>52</v>
+      <c r="C27" s="3" t="s">
+        <v>56</v>
       </c>
       <c r="D27" s="3"/>
       <c r="E27" s="3" t="s">
-        <v>38</v>
+        <v>8</v>
       </c>
     </row>
     <row r="28" ht="14.25">
@@ -1230,12 +1242,12 @@
       <c r="B28" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="C28" s="3" t="s">
-        <v>7</v>
+      <c r="C28" s="4" t="s">
+        <v>56</v>
       </c>
       <c r="D28" s="3"/>
       <c r="E28" s="3" t="s">
-        <v>8</v>
+        <v>38</v>
       </c>
     </row>
     <row r="29" ht="14.25">
@@ -1246,7 +1258,7 @@
         <v>66</v>
       </c>
       <c r="C29" s="4" t="s">
-        <v>7</v>
+        <v>56</v>
       </c>
       <c r="D29" s="3"/>
       <c r="E29" s="3" t="s">
@@ -1260,11 +1272,41 @@
       <c r="B30" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="C30" s="4" t="s">
+      <c r="C30" s="3" t="s">
         <v>7</v>
       </c>
       <c r="D30" s="3"/>
       <c r="E30" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="31" ht="14.25">
+      <c r="A31" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="B31" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="C31" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D31" s="3"/>
+      <c r="E31" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="32" ht="14.25">
+      <c r="A32" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="B32" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="C32" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D32" s="3"/>
+      <c r="E32" s="3" t="s">
         <v>38</v>
       </c>
     </row>

</xml_diff>